<commit_message>
Added nodil model Added further plot script Added further data set
</commit_message>
<xml_diff>
--- a/simulation_dataset_desc.xlsx
+++ b/simulation_dataset_desc.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="62">
   <si>
     <t>kg_vdiv_scans</t>
   </si>
@@ -49,109 +49,118 @@
     <t>standard with stress</t>
   </si>
   <si>
+    <t>kg_vdiv_K_hill_17</t>
+  </si>
+  <si>
+    <t>K_Hill</t>
+  </si>
+  <si>
+    <t>kg_vdiv_Khill_19</t>
+  </si>
+  <si>
+    <t>kg_vdiv_kpCln3_002</t>
+  </si>
+  <si>
+    <t>kpCln3</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>kg_vdiv_kpCln3_003</t>
+  </si>
+  <si>
+    <t>standard plain</t>
+  </si>
+  <si>
+    <t>kg_vdiv_kpCln3_004</t>
+  </si>
+  <si>
+    <t>kg_vdiv_kpCln3_03_kd_039</t>
+  </si>
+  <si>
+    <t>kdCln3</t>
+  </si>
+  <si>
+    <t>kg_vdiv_kpCln3_0003_kd_00039</t>
+  </si>
+  <si>
+    <t>kg_vdiv_kpCln3_0008_kd_00078</t>
+  </si>
+  <si>
+    <t>kg_vdiv_kpCln3_008_kd_0078</t>
+  </si>
+  <si>
+    <t>kg_vdiv_nHill_2</t>
+  </si>
+  <si>
+    <t>kg_vdiv_nHill_10</t>
+  </si>
+  <si>
+    <t>kg_vdiv_nHill_20</t>
+  </si>
+  <si>
+    <t>kg_vdiv_nHill_100</t>
+  </si>
+  <si>
+    <t>kg_vdiv_Whi5_50</t>
+  </si>
+  <si>
+    <t>Whi5_0</t>
+  </si>
+  <si>
+    <t>kg_vdiv_Whi5_50_st</t>
+  </si>
+  <si>
+    <t>kg_vdiv_Whi5_65_st</t>
+  </si>
+  <si>
+    <t>kg_vdiv_Whi5_100</t>
+  </si>
+  <si>
+    <t>kg_vdiv_Whi5_100_st</t>
+  </si>
+  <si>
+    <t>kg_vdiv_nodil_nHill_2</t>
+  </si>
+  <si>
+    <t>no dilution, Whi5 concentration: 2.5</t>
+  </si>
+  <si>
+    <t>kg_vdiv_nodil_nHill_15_KHill_16</t>
+  </si>
+  <si>
+    <t>no dilution, Whi5 concentration: 2.5, KHill: 1.6</t>
+  </si>
+  <si>
+    <t>kg_vdiv_nodil_nHill_10</t>
+  </si>
+  <si>
+    <t>kg_vdiv_nodil_nHill_100</t>
+  </si>
+  <si>
+    <t>kg_vdiv_nodil_plain</t>
+  </si>
+  <si>
+    <t>param_scan</t>
+  </si>
+  <si>
+    <t>varied paramters</t>
+  </si>
+  <si>
     <t>standard_with_stress</t>
   </si>
   <si>
+    <t>initial volume</t>
+  </si>
+  <si>
     <t>same as kg_vdiv_hill_coff_10, with stress as further selection for Whi3 stress plot.</t>
   </si>
   <si>
-    <t>kg_vdiv_K_hill_17</t>
-  </si>
-  <si>
-    <t>K_Hill</t>
-  </si>
-  <si>
-    <t>kg_vdiv_Khill_19</t>
-  </si>
-  <si>
-    <t>kg_vdiv_kpCln3_002</t>
-  </si>
-  <si>
-    <t>kpCln3</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>kg_vdiv_kpCln3_003</t>
-  </si>
-  <si>
-    <t>standard plain</t>
-  </si>
-  <si>
-    <t>kg_vdiv_kpCln3_004</t>
-  </si>
-  <si>
-    <t>kg_vdiv_kpCln3_03_kd_039</t>
-  </si>
-  <si>
-    <t>kdCln3</t>
-  </si>
-  <si>
-    <t>kg_vdiv_kpCln3_0003_kd_00039</t>
-  </si>
-  <si>
-    <t>kg_vdiv_kpCln3_0008_kd_00078</t>
-  </si>
-  <si>
-    <t>kg_vdiv_kpCln3_008_kd_0078</t>
-  </si>
-  <si>
-    <t>kg_vdiv_nHill_2</t>
-  </si>
-  <si>
-    <t>kg_vdiv_nHill_10</t>
-  </si>
-  <si>
-    <t>kg_vdiv_nHill_20</t>
-  </si>
-  <si>
-    <t>kg_vdiv_nHill_100</t>
-  </si>
-  <si>
-    <t>kg_vdiv_Whi5_50</t>
-  </si>
-  <si>
-    <t>Whi5_0</t>
-  </si>
-  <si>
-    <t>kg_vdiv_Whi5_50_st</t>
-  </si>
-  <si>
-    <t>kg_vdiv_Whi5_65_st</t>
-  </si>
-  <si>
-    <t>kg_vdiv_Whi5_100</t>
-  </si>
-  <si>
-    <t>kg_vdiv_Whi5_100_st</t>
-  </si>
-  <si>
-    <t>kg_vdiv_nodil_nHill_2</t>
-  </si>
-  <si>
-    <t>no dilution, Whi5 concentration: 2.5</t>
-  </si>
-  <si>
-    <t>kg_vdiv_nodil_nHill_15_KHill_16</t>
-  </si>
-  <si>
-    <t>no dilution, Whi5 concentration: 2.5, KHill: 1.6</t>
-  </si>
-  <si>
-    <t>kg_vdiv_nodil_nHill_10</t>
-  </si>
-  <si>
-    <t>kg_vdiv_nodil_nHill_100</t>
-  </si>
-  <si>
-    <t>kg_vdiv_nodil_plain</t>
-  </si>
-  <si>
-    <t>param_scan</t>
-  </si>
-  <si>
-    <t>varied paramters</t>
+    <t>n_hill_100_K_hill16_with_stress</t>
+  </si>
+  <si>
+    <t>K_Hill =1.6e6, with stress selection for stress-volume plot (Appendix)</t>
   </si>
   <si>
     <t>n_hill_1</t>
@@ -166,41 +175,35 @@
     <t>n_hill_100</t>
   </si>
   <si>
-    <t>kg_nodil_st</t>
+    <t>scan_res_vdiv_sf</t>
+  </si>
+  <si>
+    <t>scan_res_vdiv_st</t>
+  </si>
+  <si>
+    <t>scan_res_whi5_Cln3prod</t>
+  </si>
+  <si>
+    <t>used for analysis of Whi5-Cln3-Cln12 dynamics</t>
+  </si>
+  <si>
+    <t>scan_res_Whi5_Cln12prod</t>
+  </si>
+  <si>
+    <t>kpCln12</t>
+  </si>
+  <si>
+    <t>scan_res_Whi5_kg</t>
   </si>
   <si>
     <t>growth rate</t>
-  </si>
-  <si>
-    <t>kg_nodil_sf</t>
-  </si>
-  <si>
-    <t>scan_res_vdiv_sf</t>
-  </si>
-  <si>
-    <t>scan_res_vdiv_st</t>
-  </si>
-  <si>
-    <t>scan_res_whi5_Cln3prod</t>
-  </si>
-  <si>
-    <t>used for analysis of Whi5-Cln3-Cln12 dynamics</t>
-  </si>
-  <si>
-    <t>scan_res_Whi5_Cln12prod</t>
-  </si>
-  <si>
-    <t>kpCln12</t>
-  </si>
-  <si>
-    <t>scan_res_Whi5_kg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -208,17 +211,14 @@
     </font>
     <font>
       <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font/>
-    <font>
-      <b/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -296,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -313,10 +313,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -324,29 +321,27 @@
     </xf>
     <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -619,266 +614,264 @@
     </row>
     <row r="3">
       <c r="A3" s="4"/>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>9</v>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="E3" s="7">
-        <v>10.0</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>13</v>
-      </c>
+        <v>1700000.0</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="8"/>
     </row>
     <row r="4">
       <c r="A4" s="4"/>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="8">
-        <v>1700000.0</v>
+        <v>13</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1900000.0</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5">
       <c r="A5" s="4"/>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="8">
-        <v>1900000.0</v>
+      <c r="E5" s="7">
+        <v>0.002</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="9"/>
+        <v>17</v>
+      </c>
+      <c r="G5" s="8"/>
     </row>
     <row r="6">
       <c r="A6" s="4"/>
-      <c r="B6" s="7" t="s">
-        <v>17</v>
+      <c r="B6" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="8">
-        <v>0.002</v>
+        <v>16</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0.003</v>
       </c>
       <c r="F6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="9"/>
     </row>
     <row r="7">
       <c r="A7" s="4"/>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0.003</v>
+        <v>16</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.004</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>21</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="G7" s="8"/>
     </row>
     <row r="8">
       <c r="A8" s="4"/>
-      <c r="B8" s="7" t="s">
-        <v>22</v>
+      <c r="B8" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="8">
-        <v>0.004</v>
+        <v>16</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.3</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="9"/>
+        <v>17</v>
+      </c>
+      <c r="G8" s="8"/>
     </row>
     <row r="9">
       <c r="A9" s="4"/>
-      <c r="B9" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="C9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E9" s="5">
-        <v>0.3</v>
+        <v>0.39</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="9"/>
+        <v>17</v>
+      </c>
+      <c r="G9" s="8"/>
     </row>
     <row r="10">
       <c r="A10" s="4"/>
+      <c r="B10" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="C10" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="5">
-        <v>0.39</v>
+        <v>16</v>
+      </c>
+      <c r="E10" s="7">
+        <v>3.0E-4</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="9"/>
+        <v>17</v>
+      </c>
+      <c r="G10" s="8"/>
     </row>
     <row r="11">
       <c r="A11" s="4"/>
-      <c r="B11" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="C11" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="8">
-        <v>3.0E-4</v>
+        <v>22</v>
+      </c>
+      <c r="E11" s="7">
+        <v>3.9E-4</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="9"/>
+        <v>17</v>
+      </c>
+      <c r="G11" s="8"/>
     </row>
     <row r="12">
       <c r="A12" s="4"/>
+      <c r="B12" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="C12" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="8">
-        <v>3.9E-4</v>
+        <v>16</v>
+      </c>
+      <c r="E12" s="7">
+        <v>8.0E-4</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="9"/>
+        <v>17</v>
+      </c>
+      <c r="G12" s="8"/>
     </row>
     <row r="13">
       <c r="A13" s="4"/>
-      <c r="B13" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="C13" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="8">
-        <v>8.0E-4</v>
+        <v>22</v>
+      </c>
+      <c r="E13" s="7">
+        <v>7.8E-4</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="9"/>
+        <v>17</v>
+      </c>
+      <c r="G13" s="8"/>
     </row>
     <row r="14">
       <c r="A14" s="4"/>
+      <c r="B14" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="C14" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="8">
-        <v>7.8E-4</v>
+        <v>16</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0.008</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="9"/>
+        <v>17</v>
+      </c>
+      <c r="G14" s="8"/>
     </row>
     <row r="15">
       <c r="A15" s="4"/>
-      <c r="B15" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="C15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="8">
-        <v>0.008</v>
+        <v>22</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0.0078</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="9"/>
+        <v>17</v>
+      </c>
+      <c r="G15" s="8"/>
     </row>
     <row r="16">
       <c r="A16" s="4"/>
+      <c r="B16" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="C16" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="8">
-        <v>0.0078</v>
+        <v>9</v>
+      </c>
+      <c r="E16" s="5">
+        <v>2.0</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="9"/>
+        <v>10</v>
+      </c>
+      <c r="G16" s="8"/>
     </row>
     <row r="17">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>8</v>
@@ -887,17 +880,17 @@
         <v>9</v>
       </c>
       <c r="E17" s="5">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="9"/>
+      <c r="G17" s="8"/>
     </row>
     <row r="18">
       <c r="A18" s="4"/>
-      <c r="B18" s="7" t="s">
-        <v>29</v>
+      <c r="B18" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>8</v>
@@ -906,17 +899,17 @@
         <v>9</v>
       </c>
       <c r="E18" s="5">
-        <v>10.0</v>
+        <v>20.0</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="9"/>
+      <c r="G18" s="8"/>
     </row>
     <row r="19">
       <c r="A19" s="4"/>
-      <c r="B19" s="7" t="s">
-        <v>30</v>
+      <c r="B19" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>8</v>
@@ -925,130 +918,132 @@
         <v>9</v>
       </c>
       <c r="E19" s="5">
-        <v>20.0</v>
+        <v>100.0</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="9"/>
+      <c r="G19" s="8"/>
     </row>
     <row r="20">
       <c r="A20" s="4"/>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>9</v>
-      </c>
       <c r="E20" s="5">
-        <v>100.0</v>
+        <v>50.0</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="9"/>
+        <v>17</v>
+      </c>
+      <c r="G20" s="8"/>
     </row>
     <row r="21">
       <c r="A21" s="4"/>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E21" s="5">
         <v>50.0</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="9"/>
+        <v>10</v>
+      </c>
+      <c r="G21" s="8"/>
     </row>
     <row r="22">
       <c r="A22" s="4"/>
-      <c r="B22" s="7" t="s">
-        <v>34</v>
+      <c r="B22" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E22" s="5">
-        <v>50.0</v>
+        <v>65.0</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="9"/>
+      <c r="G22" s="8"/>
     </row>
     <row r="23">
       <c r="A23" s="4"/>
-      <c r="B23" s="7" t="s">
-        <v>35</v>
+      <c r="B23" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E23" s="5">
-        <v>65.0</v>
+        <v>100.0</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="9"/>
+        <v>17</v>
+      </c>
+      <c r="G23" s="8"/>
     </row>
     <row r="24">
       <c r="A24" s="4"/>
-      <c r="B24" s="7" t="s">
-        <v>36</v>
+      <c r="B24" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E24" s="5">
         <v>100.0</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="9"/>
+        <v>10</v>
+      </c>
+      <c r="G24" s="8"/>
     </row>
     <row r="25">
       <c r="A25" s="4"/>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="5">
-        <v>100.0</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25" s="9"/>
     </row>
     <row r="26">
       <c r="A26" s="4"/>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -1058,38 +1053,38 @@
         <v>9</v>
       </c>
       <c r="E26" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>10</v>
-      </c>
+        <v>15.0</v>
+      </c>
+      <c r="F26" s="5"/>
       <c r="G26" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="4"/>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="7" t="s">
+      <c r="C27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="7">
-        <v>15.0</v>
-      </c>
-      <c r="F27" s="5"/>
+      <c r="E27" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="G27" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4"/>
-      <c r="B28" s="7" t="s">
-        <v>42</v>
+      <c r="B28" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>8</v>
@@ -1098,287 +1093,282 @@
         <v>9</v>
       </c>
       <c r="E28" s="5">
+        <v>100.0</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="9"/>
+      <c r="B29" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="13"/>
+      <c r="G31" s="14"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="15"/>
+      <c r="B32" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="16">
         <v>10.0</v>
       </c>
-      <c r="F28" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="4"/>
-      <c r="B29" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="5">
-        <v>100.0</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="10"/>
-      <c r="B30" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F32" s="15"/>
-      <c r="G32" s="16"/>
+      <c r="F32" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="4"/>
-      <c r="B33" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" s="5" t="s">
+      <c r="B33" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="C33" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E33" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G33" s="9"/>
+      <c r="E33" s="16">
+        <v>100.0</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="4"/>
-      <c r="B34" s="7" t="s">
-        <v>49</v>
+      <c r="B34" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E34" s="5">
-        <v>10.0</v>
+        <v>1.0</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G34" s="9"/>
+      <c r="G34" s="8"/>
     </row>
     <row r="35">
       <c r="A35" s="4"/>
-      <c r="B35" s="7" t="s">
-        <v>50</v>
+      <c r="B35" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E35" s="5">
-        <v>100.0</v>
+        <v>10.0</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G35" s="9"/>
+      <c r="G35" s="8"/>
     </row>
     <row r="36">
       <c r="A36" s="4"/>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>52</v>
+      <c r="D36" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="5">
+        <v>100.0</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G36" s="9"/>
+      <c r="G36" s="8"/>
     </row>
     <row r="37">
       <c r="A37" s="4"/>
-      <c r="B37" s="7" t="s">
-        <v>53</v>
+      <c r="B37" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F37" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G37" s="9"/>
     </row>
     <row r="38">
       <c r="A38" s="4"/>
-      <c r="B38" s="7" t="s">
-        <v>54</v>
+      <c r="B38" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="4"/>
-      <c r="B39" s="7" t="s">
-        <v>55</v>
+      <c r="B39" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="4"/>
-      <c r="B40" s="7" t="s">
-        <v>56</v>
+      <c r="B40" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="4"/>
-      <c r="B41" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G41" s="6" t="s">
+      <c r="A41" s="9"/>
+      <c r="B41" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G41" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="10"/>
-      <c r="B42" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G42" s="13" t="s">
-        <v>57</v>
-      </c>
+    <row r="43">
+      <c r="A43" s="17"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="18"/>
+      <c r="J43" s="18"/>
+      <c r="K43" s="18"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="18"/>
+      <c r="N43" s="18"/>
+      <c r="O43" s="18"/>
+      <c r="P43" s="18"/>
+      <c r="Q43" s="18"/>
+      <c r="R43" s="18"/>
+      <c r="S43" s="18"/>
+      <c r="T43" s="18"/>
+      <c r="U43" s="18"/>
+      <c r="V43" s="18"/>
+      <c r="W43" s="18"/>
+      <c r="X43" s="18"/>
+      <c r="Y43" s="18"/>
+      <c r="Z43" s="18"/>
+      <c r="AA43" s="18"/>
     </row>
     <row r="44">
-      <c r="A44" s="17"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="19"/>
-      <c r="I44" s="19"/>
-      <c r="J44" s="19"/>
-      <c r="K44" s="19"/>
-      <c r="L44" s="19"/>
-      <c r="M44" s="19"/>
-      <c r="N44" s="19"/>
-      <c r="O44" s="19"/>
-      <c r="P44" s="19"/>
-      <c r="Q44" s="19"/>
-      <c r="R44" s="19"/>
-      <c r="S44" s="19"/>
-      <c r="T44" s="19"/>
-      <c r="U44" s="19"/>
-      <c r="V44" s="19"/>
-      <c r="W44" s="19"/>
-      <c r="X44" s="19"/>
-      <c r="Y44" s="19"/>
-      <c r="Z44" s="19"/>
-      <c r="AA44" s="19"/>
+      <c r="B44" s="19"/>
+      <c r="F44" s="20"/>
     </row>
     <row r="45">
-      <c r="B45" s="20"/>
-      <c r="F45" s="21"/>
+      <c r="B45" s="19"/>
+      <c r="F45" s="20"/>
     </row>
     <row r="46">
-      <c r="B46" s="20"/>
-      <c r="F46" s="21"/>
+      <c r="B46" s="19"/>
+      <c r="F46" s="20"/>
     </row>
     <row r="47">
-      <c r="B47" s="20"/>
-      <c r="F47" s="21"/>
+      <c r="B47" s="19"/>
+      <c r="F47" s="20"/>
     </row>
     <row r="48">
-      <c r="B48" s="20"/>
-      <c r="F48" s="21"/>
+      <c r="B48" s="19"/>
+      <c r="F48" s="20"/>
     </row>
     <row r="49">
-      <c r="B49" s="20"/>
-      <c r="F49" s="21"/>
-    </row>
-    <row r="50">
-      <c r="B50" s="20"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="21"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="20"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>